<commit_message>
SIAM - this should now be a working Module for Sessions, Identity & Access Mgt.
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="K5" authorId="0">
+    <comment ref="I20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Organization</t>
   </si>
@@ -58,24 +58,15 @@
     <t>Account</t>
   </si>
   <si>
-    <t>accPerson</t>
-  </si>
-  <si>
     <t>accUserid</t>
   </si>
   <si>
     <t>accPassword</t>
   </si>
   <si>
-    <t>accOrg</t>
-  </si>
-  <si>
     <t>accRoles</t>
   </si>
   <si>
-    <t>accOrgFunction</t>
-  </si>
-  <si>
     <t>UserID</t>
   </si>
   <si>
@@ -88,15 +79,9 @@
     <t>Role</t>
   </si>
   <si>
-    <t>OrgFunction</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
-    <t>[PersonRegistration]</t>
-  </si>
-  <si>
     <t>personFirstName</t>
   </si>
   <si>
@@ -112,9 +97,6 @@
     <t>ExcelImporter</t>
   </si>
   <si>
-    <t>autoLoginAccount</t>
-  </si>
-  <si>
     <t>ExecEngineer</t>
   </si>
   <si>
@@ -128,13 +110,88 @@
   </si>
   <si>
     <t>Administrator</t>
+  </si>
+  <si>
+    <t>accPersona</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>[OrganizationReg]</t>
+  </si>
+  <si>
+    <t>[PersonReg]</t>
+  </si>
+  <si>
+    <t>OrgAbbrName</t>
+  </si>
+  <si>
+    <t>orgAbbrName</t>
+  </si>
+  <si>
+    <t>orgFullName</t>
+  </si>
+  <si>
+    <t>OrgFullName</t>
+  </si>
+  <si>
+    <t>TNO</t>
+  </si>
+  <si>
+    <t>Organisatie voor Toegepast Wetenschappelijk Onderzoek</t>
+  </si>
+  <si>
+    <t>[Persona]</t>
+  </si>
+  <si>
+    <t>pActor</t>
+  </si>
+  <si>
+    <t>pParty</t>
+  </si>
+  <si>
+    <t>pRelation</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Rieks</t>
+  </si>
+  <si>
+    <t>Joosten</t>
+  </si>
+  <si>
+    <t>Michiel</t>
+  </si>
+  <si>
+    <t>Stornebrink</t>
+  </si>
+  <si>
+    <t>rieks</t>
+  </si>
+  <si>
+    <t>joosten</t>
+  </si>
+  <si>
+    <t>michiel</t>
+  </si>
+  <si>
+    <t>nolan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +219,16 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +240,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -184,12 +254,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -203,8 +289,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -505,31 +605,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" style="3" customWidth="1"/>
-    <col min="3" max="6" width="13.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.77734375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -537,18 +638,16 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -556,120 +655,415 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="str">
+        <f>IF($B3="","",CONCATENATE($B3," ",$C3))</f>
+        <v>Ad Minderbrood</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="str">
+        <f t="shared" ref="A4:A6" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Michiel Stornebrink</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="str">
+        <f>IF($B9="","",$B9)</f>
+        <v>TNO</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="str">
+        <f t="shared" ref="A10:A12" si="1">IF($B10="","",$B10)</f>
+        <v/>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="str">
+        <f>IF($B15="","",CONCATENATE($B15,":",$C15))</f>
+        <v>TNO:Ad Minderbrood</v>
+      </c>
+      <c r="B15" s="5" t="str">
+        <f>$A$9</f>
+        <v>TNO</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>$A3</f>
+        <v>Ad Minderbrood</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="str">
+        <f t="shared" ref="A16:A19" si="2">IF($B16="","",CONCATENATE($B16,":",$C16))</f>
+        <v>TNO:Rieks Joosten</v>
+      </c>
+      <c r="B16" s="5" t="str">
+        <f>$A$9</f>
+        <v>TNO</v>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f t="shared" ref="C16:C17" si="3">$A4</f>
+        <v>Rieks Joosten</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>TNO:Michiel Stornebrink</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f>$A$9</f>
+        <v>TNO</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Michiel Stornebrink</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <f>IF((ROWS($I$22:$I$32)-COUNTBLANK($I$22:$I$32))=0,"","autoLoginAccount")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f>$A21</f>
+        <v>Account</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="str">
+        <f>IF($D22="","",CONCATENATE("Acc_",$D22))</f>
+        <v>Acc_TNO:Ad Minderbrood</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="7" t="str">
+        <f>$A15</f>
+        <v>TNO:Ad Minderbrood</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <f>$A6</f>
-        <v>Account</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="str">
+        <f t="shared" ref="A23:A32" si="4">IF($D23="","",CONCATENATE("Acc_",$D23))</f>
+        <v>Acc_TNO:Rieks Joosten</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="7" t="str">
+        <f t="shared" ref="D23:D24" si="5">$A16</f>
+        <v>TNO:Rieks Joosten</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="F23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>Acc_TNO:Michiel Stornebrink</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>TNO:Michiel Stornebrink</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I32" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="tinus.otto@tno.nl"/>
+    <hyperlink ref="B22" r:id="rId1" display="tinus.otto@tno.nl"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
SIAM - a bit reorganized according to agreements with Michiel.
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I20" authorId="0">
+    <comment ref="J12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Organization</t>
   </si>
@@ -64,9 +64,6 @@
     <t>accPassword</t>
   </si>
   <si>
-    <t>accRoles</t>
-  </si>
-  <si>
     <t>UserID</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>ExecEngineer</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>Ad</t>
   </si>
   <si>
@@ -112,12 +106,6 @@
     <t>Administrator</t>
   </si>
   <si>
-    <t>accPersona</t>
-  </si>
-  <si>
-    <t>Persona</t>
-  </si>
-  <si>
     <t>[OrganizationReg]</t>
   </si>
   <si>
@@ -142,27 +130,6 @@
     <t>Organisatie voor Toegepast Wetenschappelijk Onderzoek</t>
   </si>
   <si>
-    <t>[Persona]</t>
-  </si>
-  <si>
-    <t>pActor</t>
-  </si>
-  <si>
-    <t>pParty</t>
-  </si>
-  <si>
-    <t>pRelation</t>
-  </si>
-  <si>
-    <t>Actor</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>Relationship</t>
-  </si>
-  <si>
     <t>Rieks</t>
   </si>
   <si>
@@ -185,6 +152,36 @@
   </si>
   <si>
     <t>nolan</t>
+  </si>
+  <si>
+    <t>accAllowedRoles</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>minderbrood</t>
+  </si>
+  <si>
+    <t>accIsGodAccount</t>
+  </si>
+  <si>
+    <t>accPerson</t>
+  </si>
+  <si>
+    <t>accOrg</t>
+  </si>
+  <si>
+    <t>Jorrit</t>
+  </si>
+  <si>
+    <t>de Boer</t>
+  </si>
+  <si>
+    <t>deboer</t>
+  </si>
+  <si>
+    <t>jorrit</t>
   </si>
 </sst>
 </file>
@@ -605,32 +602,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="3" customWidth="1"/>
+    <col min="7" max="9" width="13.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -638,16 +636,17 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -655,75 +654,71 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f>IF($B3="","",CONCATENATE($B3," ",$C3))</f>
         <v>Ad Minderbrood</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
-        <f t="shared" ref="A4:A6" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
+        <f t="shared" ref="A4:A5" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
         <v>Rieks Joosten</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Michiel Stornebrink</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="str">
+        <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
+        <v>Jorrit de Boer</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="str">
-        <f t="shared" si="0"/>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="str">
+        <f>IF($B7="","",CONCATENATE($B7," ",$C7))</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -731,342 +726,252 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="str">
-        <f>IF($B9="","",$B9)</f>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="str">
+        <f>IF($B10="","",$B10)</f>
         <v>TNO</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="str">
-        <f t="shared" ref="A10:A12" si="1">IF($B10="","",$B10)</f>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="str">
+        <f>IF($B11="","",$B11)</f>
         <v/>
       </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="str">
-        <f t="shared" si="1"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="6" t="str">
+        <f>IF((ROWS($J$14:$J$17)-COUNTBLANK($J$14:$J$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="2" t="str">
+        <f>$A13</f>
+        <v>Account</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="str">
+        <f t="shared" ref="A14:A18" si="1">IF($B14="","",CONCATENATE("Acc_",$B14))</f>
+        <v>Acc_ad</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="str">
-        <f>IF($B15="","",CONCATENATE($B15,":",$C15))</f>
-        <v>TNO:Ad Minderbrood</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <f>$A$9</f>
-        <v>TNO</v>
-      </c>
-      <c r="C15" s="3" t="str">
+      <c r="D14" s="7" t="str">
         <f>$A3</f>
         <v>Ad Minderbrood</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="str">
-        <f t="shared" ref="A16:A19" si="2">IF($B16="","",CONCATENATE($B16,":",$C16))</f>
-        <v>TNO:Rieks Joosten</v>
-      </c>
-      <c r="B16" s="5" t="str">
-        <f>$A$9</f>
+      <c r="E14" s="7" t="str">
+        <f>$A$10</f>
         <v>TNO</v>
       </c>
-      <c r="C16" s="3" t="str">
-        <f t="shared" ref="C16:C17" si="3">$A4</f>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Acc_rieks</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="str">
+        <f t="shared" ref="D15" si="2">$A4</f>
         <v>Rieks Joosten</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>TNO:Michiel Stornebrink</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <f>$A$9</f>
+      <c r="E15" s="7" t="str">
+        <f t="shared" ref="E15:E18" si="3">$A$10</f>
         <v>TNO</v>
       </c>
-      <c r="C17" s="3" t="str">
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" t="str">
+        <f>$A15</f>
+        <v>Acc_rieks</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Acc_michiel</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="7" t="str">
+        <f t="shared" ref="D16" si="4">$A5</f>
+        <v>Michiel Stornebrink</v>
+      </c>
+      <c r="E16" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>Michiel Stornebrink</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="str">
-        <f t="shared" si="2"/>
+        <v>TNO</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Acc_jorrit</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f>$A6</f>
+        <v>Jorrit de Boer</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>TNO</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="str">
+        <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="str">
-        <f t="shared" si="2"/>
+      <c r="D18" s="7" t="str">
+        <f>$A7</f>
         <v/>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" s="6" t="str">
-        <f>IF((ROWS($I$22:$I$32)-COUNTBLANK($I$22:$I$32))=0,"","autoLoginAccount")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="2" t="str">
-        <f>$A21</f>
-        <v>Account</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="str">
-        <f>IF($D22="","",CONCATENATE("Acc_",$D22))</f>
-        <v>Acc_TNO:Ad Minderbrood</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="7" t="str">
-        <f>$A15</f>
-        <v>TNO:Ad Minderbrood</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="str">
-        <f t="shared" ref="A23:A32" si="4">IF($D23="","",CONCATENATE("Acc_",$D23))</f>
-        <v>Acc_TNO:Rieks Joosten</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f t="shared" ref="D23:D24" si="5">$A16</f>
-        <v>TNO:Rieks Joosten</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>Acc_TNO:Michiel Stornebrink</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>TNO:Michiel Stornebrink</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I32" s="7"/>
+      <c r="E18" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>TNO</v>
+      </c>
+      <c r="J18" s="7"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" display="tinus.otto@tno.nl"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SIAM - major revision of structure, leaving the functionality as it was before
Changes (that I remember)
- Added CRUD-stuff to INTERFACEs
- New feature: versioning
- New feature: ISO levels of assurance/authentication
- Existing features, i.e. GodAccounts, auto login, and session suspension have been split out to separate files, allowing developers not to use them.
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="J12" authorId="0">
+    <comment ref="G12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Organization</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Person</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -91,21 +88,12 @@
     <t>personLastName</t>
   </si>
   <si>
-    <t>ExcelImporter</t>
-  </si>
-  <si>
-    <t>ExecEngineer</t>
-  </si>
-  <si>
     <t>Ad</t>
   </si>
   <si>
     <t>Minderbrood</t>
   </si>
   <si>
-    <t>Administrator</t>
-  </si>
-  <si>
     <t>[OrganizationReg]</t>
   </si>
   <si>
@@ -182,6 +170,15 @@
   </si>
   <si>
     <t>jorrit</t>
+  </si>
+  <si>
+    <t>User, Administrator</t>
+  </si>
+  <si>
+    <t>User, Administrator, ExcelImporter, ExecEngineer</t>
+  </si>
+  <si>
+    <t>[Role,]</t>
   </si>
 </sst>
 </file>
@@ -602,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I12" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,152 +611,139 @@
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" style="3" customWidth="1"/>
-    <col min="7" max="9" width="13.77734375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f>IF($B3="","",CONCATENATE($B3," ",$C3))</f>
         <v>Ad Minderbrood</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f t="shared" ref="A4:A5" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
         <v>Rieks Joosten</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Michiel Stornebrink</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
         <v>Jorrit de Boer</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f>IF($B7="","",CONCATENATE($B7," ",$C7))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>TNO</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f>IF($B11="","",$B11)</f>
         <v/>
@@ -767,7 +751,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -778,32 +762,23 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="6" t="str">
-        <f>IF((ROWS($J$14:$J$17)-COUNTBLANK($J$14:$J$17))=0,"","autoLoginAccount")</f>
+        <v>31</v>
+      </c>
+      <c r="G12" s="6" t="str">
+        <f>IF((ROWS($G$14:$G$17)-COUNTBLANK($G$14:$G$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -820,35 +795,26 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="2" t="str">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2" t="str">
         <f>$A13</f>
         <v>Account</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
-        <f t="shared" ref="A14:A18" si="1">IF($B14="","",CONCATENATE("Acc_",$B14))</f>
+        <f t="shared" ref="A14:A17" si="1">IF($B14="","",CONCATENATE("Acc_",$B14))</f>
         <v>Acc_ad</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D14" s="7" t="str">
         <f>$A3</f>
@@ -859,29 +825,20 @@
         <v>TNO</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_rieks</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="str">
         <f t="shared" ref="D15" si="2">$A4</f>
@@ -892,27 +849,24 @@
         <v>TNO</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" t="str">
+        <v>41</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" t="str">
         <f>$A15</f>
         <v>Acc_rieks</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_michiel</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="7" t="str">
         <f t="shared" ref="D16" si="4">$A5</f>
@@ -923,23 +877,20 @@
         <v>TNO</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_jorrit</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" s="7" t="str">
         <f>$A6</f>
@@ -949,12 +900,12 @@
         <f t="shared" si="3"/>
         <v>TNO</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
@@ -967,7 +918,7 @@
         <f t="shared" si="3"/>
         <v>TNO</v>
       </c>
-      <c r="J18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SIAM - updated documentation to v2.1, ISOLevels are INTEGERs now (rather than 'real' atoms)
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="G12" authorId="0">
+    <comment ref="H12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Organization</t>
   </si>
@@ -175,17 +175,77 @@
     <t>User, Administrator</t>
   </si>
   <si>
-    <t>User, Administrator, ExcelImporter, ExecEngineer</t>
-  </si>
-  <si>
     <t>[Role,]</t>
+  </si>
+  <si>
+    <t>[UIDs]</t>
+  </si>
+  <si>
+    <t>Administrator, ExcelImporter, ExecEngineer</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>accUID</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>uidIdP</t>
+  </si>
+  <si>
+    <t>uidUserid</t>
+  </si>
+  <si>
+    <t>google.com</t>
+  </si>
+  <si>
+    <t>ms@g</t>
+  </si>
+  <si>
+    <t>[UID,]</t>
+  </si>
+  <si>
+    <t>ms@g, ms@li</t>
+  </si>
+  <si>
+    <t>ms@li</t>
+  </si>
+  <si>
+    <t>linkedin.com</t>
+  </si>
+  <si>
+    <t>IdP</t>
+  </si>
+  <si>
+    <t>rj@g, rj@tno</t>
+  </si>
+  <si>
+    <t>ms@tno</t>
+  </si>
+  <si>
+    <t>tno.nl</t>
+  </si>
+  <si>
+    <t>stornebrinkm</t>
+  </si>
+  <si>
+    <t>rj@tno</t>
+  </si>
+  <si>
+    <t>joostenhjm</t>
+  </si>
+  <si>
+    <t>rj@g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +277,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -264,12 +332,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -296,9 +365,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -599,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:I13"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,13 +688,13 @@
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="45.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -630,8 +708,9 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -645,8 +724,9 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f>IF($B3="","",CONCATENATE($B3," ",$C3))</f>
         <v>Ad Minderbrood</v>
@@ -658,7 +738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f t="shared" ref="A4:A5" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
         <v>Rieks Joosten</v>
@@ -670,7 +750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Michiel Stornebrink</v>
@@ -682,7 +762,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
         <v>Jorrit de Boer</v>
@@ -694,13 +774,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f>IF($B7="","",CONCATENATE($B7," ",$C7))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -714,8 +794,9 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -729,8 +810,9 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>TNO</v>
@@ -743,7 +825,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f>IF($B11="","",$B11)</f>
         <v/>
@@ -751,7 +833,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -768,17 +850,20 @@
         <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="6" t="str">
-        <f>IF((ROWS($G$14:$G$17)-COUNTBLANK($G$14:$G$17))=0,"","autoLoginAccount")</f>
+      <c r="H12" s="6" t="str">
+        <f>IF((ROWS($H$14:$H$17)-COUNTBLANK($H$14:$H$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -795,17 +880,20 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="2" t="str">
+        <v>52</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="2" t="str">
         <f>$A13</f>
         <v>Account</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
         <f t="shared" ref="A14:A17" si="1">IF($B14="","",CONCATENATE("Acc_",$B14))</f>
         <v>Acc_ad</v>
@@ -824,12 +912,12 @@
         <f>$A$10</f>
         <v>TNO</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_rieks</v>
@@ -849,15 +937,18 @@
         <v>TNO</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" t="str">
+        <v>57</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" t="str">
         <f>$A15</f>
         <v>Acc_rieks</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_michiel</v>
@@ -877,11 +968,14 @@
         <v>TNO</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_jorrit</v>
@@ -900,12 +994,12 @@
         <f t="shared" si="3"/>
         <v>TNO</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
@@ -918,11 +1012,106 @@
         <f t="shared" si="3"/>
         <v>TNO</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="20" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A22" r:id="rId1"/>
+    <hyperlink ref="F16" r:id="rId2" display="ms@google"/>
+    <hyperlink ref="A23" r:id="rId3"/>
+    <hyperlink ref="A24" r:id="rId4"/>
+    <hyperlink ref="A25" r:id="rId5"/>
+    <hyperlink ref="A26" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SIAM - Added account initialization/activation; PLEASE MAKE SURE YOU INCLUDE RULE `Account activation/initialization` (from SIAM_Module-example.adl) IN YOUR OWN ADL FILES!
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Organization</t>
   </si>
@@ -133,24 +133,15 @@
     <t>rieks</t>
   </si>
   <si>
-    <t>joosten</t>
-  </si>
-  <si>
     <t>michiel</t>
   </si>
   <si>
-    <t>nolan</t>
-  </si>
-  <si>
     <t>accAllowedRoles</t>
   </si>
   <si>
     <t>ad</t>
   </si>
   <si>
-    <t>minderbrood</t>
-  </si>
-  <si>
     <t>accIsGodAccount</t>
   </si>
   <si>
@@ -160,18 +151,6 @@
     <t>accOrg</t>
   </si>
   <si>
-    <t>Jorrit</t>
-  </si>
-  <si>
-    <t>de Boer</t>
-  </si>
-  <si>
-    <t>deboer</t>
-  </si>
-  <si>
-    <t>jorrit</t>
-  </si>
-  <si>
     <t>User, Administrator</t>
   </si>
   <si>
@@ -239,6 +218,15 @@
   </si>
   <si>
     <t>rj@g</t>
+  </si>
+  <si>
+    <t>Jelle</t>
+  </si>
+  <si>
+    <t>Nauta</t>
+  </si>
+  <si>
+    <t>jelle</t>
   </si>
 </sst>
 </file>
@@ -677,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,13 +753,13 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
-        <v>Jorrit de Boer</v>
+        <v>Jelle Nauta</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -844,23 +832,23 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12" s="6" t="str">
         <f>IF((ROWS($H$14:$H$17)-COUNTBLANK($H$14:$H$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
       <c r="I12" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -880,10 +868,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>$A13</f>
@@ -899,21 +887,22 @@
         <v>Acc_ad</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="str">
+        <f>IF($B14="","","*****")</f>
+        <v>*****</v>
       </c>
       <c r="D14" s="7" t="str">
         <f>$A3</f>
         <v>Ad Minderbrood</v>
       </c>
       <c r="E14" s="7" t="str">
-        <f>$A$10</f>
+        <f>IF($B14="","",$A$10)</f>
         <v>TNO</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H14" s="7"/>
     </row>
@@ -925,22 +914,23 @@
       <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
+      <c r="C15" s="7" t="str">
+        <f t="shared" ref="C15:C18" si="2">IF($B15="","","*****")</f>
+        <v>*****</v>
       </c>
       <c r="D15" s="7" t="str">
-        <f t="shared" ref="D15" si="2">$A4</f>
+        <f t="shared" ref="D15" si="3">$A4</f>
         <v>Rieks Joosten</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f t="shared" ref="E15:E18" si="3">$A$10</f>
+        <f t="shared" ref="E15:E18" si="4">IF($B15="","",$A$10)</f>
         <v>TNO</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" t="str">
@@ -954,44 +944,46 @@
         <v>Acc_michiel</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>*****</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f t="shared" ref="D16" si="4">$A5</f>
+        <f t="shared" ref="D16" si="5">$A5</f>
         <v>Michiel Stornebrink</v>
       </c>
       <c r="E16" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TNO</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>Acc_jorrit</v>
+        <v>Acc_jelle</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>*****</v>
       </c>
       <c r="D17" s="7" t="str">
         <f>$A6</f>
-        <v>Jorrit de Boer</v>
+        <v>Jelle Nauta</v>
       </c>
       <c r="E17" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>TNO</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1004,25 +996,45 @@
         <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
       </c>
+      <c r="C18" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="D18" s="7" t="str">
         <f>$A7</f>
         <v/>
       </c>
       <c r="E18" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>TNO</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1030,85 +1042,69 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1"/>
+    <hyperlink ref="A21" r:id="rId1"/>
     <hyperlink ref="F16" r:id="rId2" display="ms@google"/>
-    <hyperlink ref="A23" r:id="rId3"/>
-    <hyperlink ref="A24" r:id="rId4"/>
-    <hyperlink ref="A25" r:id="rId5"/>
-    <hyperlink ref="A26" r:id="rId6"/>
+    <hyperlink ref="A22" r:id="rId3"/>
+    <hyperlink ref="A23" r:id="rId4"/>
+    <hyperlink ref="A24" r:id="rId5"/>
+    <hyperlink ref="A25" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
SIAM - Atomic references syntax adjusted for Ampersand v3.9.0 (24 november 2017) (See issue #724)
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I12" authorId="0">
+    <comment ref="H12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Organization</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>jelle</t>
-  </si>
-  <si>
-    <t>accIsActive</t>
   </si>
 </sst>
 </file>
@@ -668,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,7 +682,7 @@
     <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -701,7 +698,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -717,7 +714,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f>IF($B3="","",CONCATENATE($B3," ",$C3))</f>
         <v>Ad Minderbrood</v>
@@ -729,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f t="shared" ref="A4:A5" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
         <v>Rieks Joosten</v>
@@ -741,7 +738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Michiel Stornebrink</v>
@@ -753,7 +750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
         <v>Jelle Nauta</v>
@@ -765,13 +762,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f>IF($B7="","",CONCATENATE($B7," ",$C7))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -787,7 +784,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +800,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>TNO</v>
@@ -816,7 +813,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f>IF($B11="","",$B11)</f>
         <v/>
@@ -824,224 +821,196 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>60</v>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="6" t="str">
-        <f>IF((ROWS($I$14:$I$17)-COUNTBLANK($I$14:$I$17))=0,"","autoLoginAccount")</f>
+      <c r="H12" s="6" t="str">
+        <f>IF((ROWS($H$14:$H$17)-COUNTBLANK($H$14:$H$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="str">
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="2" t="str">
         <f>$A13</f>
         <v>Account</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <f>$A13</f>
-        <v>Account</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
-        <f t="shared" ref="A14:A17" si="1">IF($C14="","",CONCATENATE("Acc_",$C14))</f>
+        <f t="shared" ref="A14:A17" si="1">IF($B14="","",CONCATENATE("Acc_",$B14))</f>
         <v>Acc_ad</v>
       </c>
-      <c r="B14" s="8" t="str">
-        <f>$A14</f>
-        <v>Acc_ad</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C14" s="7" t="str">
+        <f>IF($B14="","","*****")</f>
+        <v>*****</v>
+      </c>
       <c r="D14" s="7" t="str">
-        <f>IF($C14="","","*****")</f>
-        <v>*****</v>
-      </c>
-      <c r="E14" s="7" t="str">
         <f>$A3</f>
         <v>Ad Minderbrood</v>
       </c>
-      <c r="F14" s="7" t="str">
-        <f>IF($C14="","",$A$10)</f>
+      <c r="E14" s="7" t="str">
+        <f>IF($B14="","",$A$10)</f>
         <v>TNO</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_rieks</v>
       </c>
-      <c r="B15" s="8" t="str">
-        <f t="shared" ref="B15:B18" si="2">$A15</f>
-        <v>Acc_rieks</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="C15" s="7" t="str">
+        <f t="shared" ref="C15:C18" si="2">IF($B15="","","*****")</f>
+        <v>*****</v>
+      </c>
       <c r="D15" s="7" t="str">
-        <f t="shared" ref="D15:D18" si="3">IF($C15="","","*****")</f>
-        <v>*****</v>
+        <f t="shared" ref="D15" si="3">$A4</f>
+        <v>Rieks Joosten</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f t="shared" ref="E15" si="4">$A4</f>
-        <v>Rieks Joosten</v>
-      </c>
-      <c r="F15" s="7" t="str">
-        <f>IF($C15="","",$A$10)</f>
+        <f t="shared" ref="E15:E18" si="4">IF($B15="","",$A$10)</f>
         <v>TNO</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" t="str">
+      <c r="H15" s="7"/>
+      <c r="I15" t="str">
         <f>$A15</f>
         <v>Acc_rieks</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_michiel</v>
       </c>
-      <c r="B16" s="8" t="str">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_michiel</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>*****</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>*****</v>
+        <f t="shared" ref="D16" si="5">$A5</f>
+        <v>Michiel Stornebrink</v>
       </c>
       <c r="E16" s="7" t="str">
-        <f t="shared" ref="E16" si="5">$A5</f>
-        <v>Michiel Stornebrink</v>
-      </c>
-      <c r="F16" s="7" t="str">
-        <f>IF($C16="","",$A$10)</f>
+        <f t="shared" si="4"/>
         <v>TNO</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_jelle</v>
       </c>
-      <c r="B17" s="8" t="str">
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_jelle</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>59</v>
+        <v>*****</v>
       </c>
       <c r="D17" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>*****</v>
-      </c>
-      <c r="E17" s="7" t="str">
         <f>$A6</f>
         <v>Jelle Nauta</v>
       </c>
-      <c r="F17" s="7" t="str">
-        <f>IF($C17="","",$A$10)</f>
+      <c r="E17" s="7" t="str">
+        <f t="shared" si="4"/>
         <v>TNO</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
-        <f>IF($C18="","",CONCATENATE("Acc_",$C18))</f>
+        <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
       </c>
-      <c r="B18" s="8" t="str">
+      <c r="C18" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C18" s="5"/>
       <c r="D18" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E18" s="7" t="str">
         <f>$A7</f>
         <v/>
       </c>
-      <c r="F18" s="7" t="str">
-        <f>IF($C18="","",$A$10)</f>
+      <c r="E18" s="7" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>36</v>
       </c>
@@ -1057,7 +1026,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>40</v>
       </c>
@@ -1073,7 +1042,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>44</v>
       </c>
@@ -1084,7 +1053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>47</v>
       </c>
@@ -1095,7 +1064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
@@ -1106,7 +1075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>54</v>
       </c>
@@ -1117,7 +1086,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>56</v>
       </c>
@@ -1131,7 +1100,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="G16" r:id="rId2" display="ms@google"/>
+    <hyperlink ref="F16" r:id="rId2" display="ms@google"/>
     <hyperlink ref="A22" r:id="rId3"/>
     <hyperlink ref="A23" r:id="rId4"/>
     <hyperlink ref="A24" r:id="rId5"/>

</xml_diff>

<commit_message>
SIAM - further adaptions to accommodate refactoring
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I12" authorId="0">
+    <comment ref="H12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Organization</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>jelle</t>
-  </si>
-  <si>
-    <t>accIsActive</t>
   </si>
 </sst>
 </file>
@@ -668,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,7 +682,7 @@
     <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -701,7 +698,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -717,7 +714,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f>IF($B3="","",CONCATENATE($B3," ",$C3))</f>
         <v>Ad Minderbrood</v>
@@ -729,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f t="shared" ref="A4:A5" si="0">IF($B4="","",CONCATENATE($B4," ",$C4))</f>
         <v>Rieks Joosten</v>
@@ -741,7 +738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Michiel Stornebrink</v>
@@ -753,7 +750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
         <v>Jelle Nauta</v>
@@ -765,13 +762,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f>IF($B7="","",CONCATENATE($B7," ",$C7))</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -787,7 +784,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +800,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>TNO</v>
@@ -816,7 +813,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f>IF($B11="","",$B11)</f>
         <v/>
@@ -824,224 +821,196 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>60</v>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="6" t="str">
-        <f>IF((ROWS($I$14:$I$17)-COUNTBLANK($I$14:$I$17))=0,"","autoLoginAccount")</f>
+      <c r="H12" s="6" t="str">
+        <f>IF((ROWS($H$14:$H$17)-COUNTBLANK($H$14:$H$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="str">
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="2" t="str">
         <f>$A13</f>
         <v>Account</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <f>$A13</f>
-        <v>Account</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="str">
-        <f t="shared" ref="A14:A17" si="1">IF($C14="","",CONCATENATE("Acc_",$C14))</f>
+        <f t="shared" ref="A14:A17" si="1">IF($B14="","",CONCATENATE("Acc_",$B14))</f>
         <v>Acc_ad</v>
       </c>
-      <c r="B14" s="8" t="str">
-        <f>$A14</f>
-        <v>Acc_ad</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C14" s="7" t="str">
+        <f>IF($B14="","","*****")</f>
+        <v>*****</v>
+      </c>
       <c r="D14" s="7" t="str">
-        <f>IF($C14="","","*****")</f>
-        <v>*****</v>
-      </c>
-      <c r="E14" s="7" t="str">
         <f>$A3</f>
         <v>Ad Minderbrood</v>
       </c>
-      <c r="F14" s="7" t="str">
-        <f>IF($C14="","",$A$10)</f>
+      <c r="E14" s="7" t="str">
+        <f>IF($B14="","",$A$10)</f>
         <v>TNO</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_rieks</v>
       </c>
-      <c r="B15" s="8" t="str">
-        <f t="shared" ref="B15:B18" si="2">$A15</f>
-        <v>Acc_rieks</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="C15" s="7" t="str">
+        <f t="shared" ref="C15:C18" si="2">IF($B15="","","*****")</f>
+        <v>*****</v>
+      </c>
       <c r="D15" s="7" t="str">
-        <f t="shared" ref="D15:D18" si="3">IF($C15="","","*****")</f>
-        <v>*****</v>
+        <f t="shared" ref="D15" si="3">$A4</f>
+        <v>Rieks Joosten</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f t="shared" ref="E15" si="4">$A4</f>
-        <v>Rieks Joosten</v>
-      </c>
-      <c r="F15" s="7" t="str">
-        <f>IF($C15="","",$A$10)</f>
+        <f t="shared" ref="E15:E18" si="4">IF($B15="","",$A$10)</f>
         <v>TNO</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" t="str">
+      <c r="H15" s="7"/>
+      <c r="I15" t="str">
         <f>$A15</f>
         <v>Acc_rieks</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_michiel</v>
       </c>
-      <c r="B16" s="8" t="str">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_michiel</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>*****</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>*****</v>
+        <f t="shared" ref="D16" si="5">$A5</f>
+        <v>Michiel Stornebrink</v>
       </c>
       <c r="E16" s="7" t="str">
-        <f t="shared" ref="E16" si="5">$A5</f>
-        <v>Michiel Stornebrink</v>
-      </c>
-      <c r="F16" s="7" t="str">
-        <f>IF($C16="","",$A$10)</f>
+        <f t="shared" si="4"/>
         <v>TNO</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Acc_jelle</v>
       </c>
-      <c r="B17" s="8" t="str">
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_jelle</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>59</v>
+        <v>*****</v>
       </c>
       <c r="D17" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>*****</v>
-      </c>
-      <c r="E17" s="7" t="str">
         <f>$A6</f>
         <v>Jelle Nauta</v>
       </c>
-      <c r="F17" s="7" t="str">
-        <f>IF($C17="","",$A$10)</f>
+      <c r="E17" s="7" t="str">
+        <f t="shared" si="4"/>
         <v>TNO</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
-        <f>IF($C18="","",CONCATENATE("Acc_",$C18))</f>
+        <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
       </c>
-      <c r="B18" s="8" t="str">
+      <c r="C18" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C18" s="5"/>
       <c r="D18" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E18" s="7" t="str">
         <f>$A7</f>
         <v/>
       </c>
-      <c r="F18" s="7" t="str">
-        <f>IF($C18="","",$A$10)</f>
+      <c r="E18" s="7" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>36</v>
       </c>
@@ -1057,7 +1026,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>40</v>
       </c>
@@ -1073,7 +1042,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>44</v>
       </c>
@@ -1084,7 +1053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>47</v>
       </c>
@@ -1095,7 +1064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
@@ -1106,7 +1075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>54</v>
       </c>
@@ -1117,7 +1086,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>56</v>
       </c>
@@ -1131,7 +1100,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A21" r:id="rId1"/>
-    <hyperlink ref="G16" r:id="rId2" display="ms@google"/>
+    <hyperlink ref="F16" r:id="rId2" display="ms@google"/>
     <hyperlink ref="A22" r:id="rId3"/>
     <hyperlink ref="A23" r:id="rId4"/>
     <hyperlink ref="A24" r:id="rId5"/>

</xml_diff>